<commit_message>
dashboard and search function
</commit_message>
<xml_diff>
--- a/douments/check list.xlsx
+++ b/douments/check list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\bit\douments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36713BB-11E8-4CA0-B434-3C403D06789A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85422452-8F1C-4D05-A905-CE0DD325D119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="34560" windowHeight="18600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Update Quary Error at spec_items tabel</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>item sepcifications values retrive</t>
+  </si>
+  <si>
+    <t>item update with out changing the name</t>
   </si>
 </sst>
 </file>
@@ -367,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="295" zoomScaleNormal="295" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -404,6 +407,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>